<commit_message>
[DEMO] Updated seeding file
</commit_message>
<xml_diff>
--- a/demo-artifacts/post.xlsx
+++ b/demo-artifacts/post.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/184ac7bbb05968eb/Bureaublad/pxl_2024/fullStack_java/PXLNews_seed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suzen\source\repos\project-Su-zenGeurtsPXL-1\demo-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{CADA5B5F-03BA-48FF-A10F-947040D40B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E68CB62-2AEE-40F8-B0F2-FE536C5CC611}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886F25FE-0246-44DB-A2FA-90FDD1A24967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -643,10 +643,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -967,7 +963,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G2" sqref="G2:G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1018,7 +1014,7 @@
       </c>
       <c r="D2" s="3">
         <f ca="1">RANDBETWEEN(DATE(2024,12,0),DATE(2024,12,31))+RANDBETWEEN(TIME(8,0,0)*10000,TIME(17,0,0)*10000)/10000</f>
-        <v>45633.669300000001</v>
+        <v>45636.6728</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1043,7 +1039,7 @@
       </c>
       <c r="D3" s="3">
         <f t="shared" ref="D3:D6" ca="1" si="0">RANDBETWEEN(DATE(2024,12,0),DATE(2024,12,31))+RANDBETWEEN(TIME(8,0,0)*10000,TIME(17,0,0)*10000)/10000</f>
-        <v>45643.533199999998</v>
+        <v>45635.428999999996</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1068,7 +1064,7 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45653.523099999999</v>
+        <v>45642.4427</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1093,7 +1089,7 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45657.351699999999</v>
+        <v>45638.389199999998</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1108,7 +1104,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1118,7 +1114,7 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45627.699200000003</v>
+        <v>45638.363100000002</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1127,24 +1123,24 @@
         <v>16</v>
       </c>
       <c r="G6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <f ca="1">RANDBETWEEN(0,6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="3">
         <f ca="1">RANDBETWEEN(DATE(2022,9,31),DATE(2024,11,30))+RANDBETWEEN(TIME(8,0,0)*10000,TIME(17,0,0)*10000)/10000</f>
-        <v>45255.3465</v>
+        <v>45233.646500000003</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1153,25 +1149,24 @@
         <v>17</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G65" ca="1" si="1">RANDBETWEEN(1,7)</f>
         <v>6</v>
       </c>
       <c r="K7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B71" ca="1" si="2">RANDBETWEEN(0,6)</f>
-        <v>3</v>
+        <f t="shared" ref="B8:B71" ca="1" si="1">RANDBETWEEN(0,6)</f>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" ref="D8:D71" ca="1" si="3">RANDBETWEEN(DATE(2022,9,31),DATE(2024,11,30))+RANDBETWEEN(TIME(8,0,0)*10000,TIME(17,0,0)*10000)/10000</f>
-        <v>44845.612999999998</v>
+        <f t="shared" ref="D8:D71" ca="1" si="2">RANDBETWEEN(DATE(2022,9,31),DATE(2024,11,30))+RANDBETWEEN(TIME(8,0,0)*10000,TIME(17,0,0)*10000)/10000</f>
+        <v>45003.658000000003</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1180,25 +1175,24 @@
         <v>17</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44902.423799999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45490.427900000002</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1207,25 +1201,24 @@
         <v>17</v>
       </c>
       <c r="G9">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44925.511299999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45152.555200000003</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1234,25 +1227,24 @@
         <v>17</v>
       </c>
       <c r="G10">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45277.618499999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45381.6783</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1261,25 +1253,24 @@
         <v>17</v>
       </c>
       <c r="G11">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45173.3485</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45212.454400000002</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1288,25 +1279,24 @@
         <v>17</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45612.657500000001</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45111.504999999997</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -1315,25 +1305,24 @@
         <v>17</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K13"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45313.453099999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45368.563699999999</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1342,25 +1331,24 @@
         <v>17</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="K14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45357.619200000001</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45141.645299999996</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -1369,25 +1357,24 @@
         <v>17</v>
       </c>
       <c r="G15">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="K15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45213.421600000001</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45566.579700000002</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1396,25 +1383,24 @@
         <v>17</v>
       </c>
       <c r="G16">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K16"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45451.359499999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45384.613899999997</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1423,25 +1409,24 @@
         <v>17</v>
       </c>
       <c r="G17">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K17"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45467.377</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45034.684500000003</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -1450,25 +1435,24 @@
         <v>17</v>
       </c>
       <c r="G18">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45332.424299999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44956.535300000003</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -1477,25 +1461,24 @@
         <v>17</v>
       </c>
       <c r="G19">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45104.4539</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45514.399599999997</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -1504,25 +1487,24 @@
         <v>17</v>
       </c>
       <c r="G20">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="K20"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45562.612500000003</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44908.351300000002</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1531,25 +1513,24 @@
         <v>17</v>
       </c>
       <c r="G21">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45062.357600000003</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45604.4931</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1558,25 +1539,24 @@
         <v>17</v>
       </c>
       <c r="G22">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="K22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45226.663999999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45463.563399999999</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1585,25 +1565,24 @@
         <v>17</v>
       </c>
       <c r="G23">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K23"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45125.474099999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45243.569100000001</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -1612,25 +1591,24 @@
         <v>17</v>
       </c>
       <c r="G24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="K24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44987.6175</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45381.4257</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1639,25 +1617,24 @@
         <v>17</v>
       </c>
       <c r="G25">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="K25"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45072.587</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44922.656199999998</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1666,25 +1643,24 @@
         <v>17</v>
       </c>
       <c r="G26">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="K26"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45366.486400000002</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45477.434999999998</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1693,25 +1669,24 @@
         <v>17</v>
       </c>
       <c r="G27">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="K27"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45353.522400000002</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45573.590700000001</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -1720,25 +1695,24 @@
         <v>17</v>
       </c>
       <c r="G28">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="K28"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45016.573199999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45410.466200000003</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -1747,25 +1721,24 @@
         <v>17</v>
       </c>
       <c r="G29">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="K29"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44853.694100000001</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45254.457000000002</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -1774,25 +1747,24 @@
         <v>17</v>
       </c>
       <c r="G30">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="K30"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45511.542800000003</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45113.618600000002</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -1801,25 +1773,24 @@
         <v>17</v>
       </c>
       <c r="G31">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="K31"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45459.589200000002</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44973.626300000004</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -1828,25 +1799,24 @@
         <v>17</v>
       </c>
       <c r="G32">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="K32"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45516.570899999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45279.539700000001</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -1855,25 +1825,24 @@
         <v>17</v>
       </c>
       <c r="G33">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="K33"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44943.7016</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45372.663500000002</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -1882,25 +1851,24 @@
         <v>17</v>
       </c>
       <c r="G34">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="K34"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45232.399599999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45014.525800000003</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -1909,25 +1877,24 @@
         <v>17</v>
       </c>
       <c r="G35">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="K35"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44902.464</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45261.633900000001</v>
       </c>
       <c r="E36">
         <v>2</v>
@@ -1936,25 +1903,24 @@
         <v>17</v>
       </c>
       <c r="G36">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="K36"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44887.411699999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45067.414400000001</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1963,25 +1929,24 @@
         <v>17</v>
       </c>
       <c r="G37">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="K37"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44856.629399999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45053.690399999999</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -1990,25 +1955,24 @@
         <v>17</v>
       </c>
       <c r="G38">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="K38"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45010.4611</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45296.572800000002</v>
       </c>
       <c r="E39">
         <v>2</v>
@@ -2017,25 +1981,24 @@
         <v>17</v>
       </c>
       <c r="G39">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="K39"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45392.494599999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45036.481200000002</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -2044,25 +2007,24 @@
         <v>17</v>
       </c>
       <c r="G40">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="K40"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45424.427199999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44850.614399999999</v>
       </c>
       <c r="E41">
         <v>2</v>
@@ -2071,25 +2033,24 @@
         <v>17</v>
       </c>
       <c r="G41">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="K41"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45007.411599999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44965.643100000001</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -2098,25 +2059,24 @@
         <v>17</v>
       </c>
       <c r="G42">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="K42"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45181.605300000003</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45298.389000000003</v>
       </c>
       <c r="E43">
         <v>2</v>
@@ -2125,25 +2085,24 @@
         <v>17</v>
       </c>
       <c r="G43">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="K43"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45181.343099999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45031.489099999999</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -2152,25 +2111,24 @@
         <v>17</v>
       </c>
       <c r="G44">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="K44"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45076.654499999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44928.632100000003</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -2179,25 +2137,24 @@
         <v>17</v>
       </c>
       <c r="G45">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="K45"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45313.549099999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45259.701800000003</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -2206,25 +2163,24 @@
         <v>17</v>
       </c>
       <c r="G46">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="K46"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44927.394800000002</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45573.640899999999</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -2233,25 +2189,24 @@
         <v>17</v>
       </c>
       <c r="G47">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="K47"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45558.575199999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45083.496599999999</v>
       </c>
       <c r="E48">
         <v>2</v>
@@ -2260,25 +2215,24 @@
         <v>17</v>
       </c>
       <c r="G48">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="K48"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45109.595699999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45281.367700000003</v>
       </c>
       <c r="E49">
         <v>2</v>
@@ -2287,25 +2241,24 @@
         <v>17</v>
       </c>
       <c r="G49">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="K49"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45565.373299999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45186.557500000003</v>
       </c>
       <c r="E50">
         <v>2</v>
@@ -2314,25 +2267,24 @@
         <v>17</v>
       </c>
       <c r="G50">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="K50"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45140.698199999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45525.336499999998</v>
       </c>
       <c r="E51">
         <v>2</v>
@@ -2341,25 +2293,24 @@
         <v>17</v>
       </c>
       <c r="G51">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="K51"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C52" t="s">
         <v>17</v>
       </c>
       <c r="D52" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45357.682699999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45453.419699999999</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -2368,25 +2319,24 @@
         <v>17</v>
       </c>
       <c r="G52">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="K52"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
         <v>17</v>
       </c>
       <c r="D53" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45093.407500000001</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45172.412900000003</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -2395,25 +2345,24 @@
         <v>17</v>
       </c>
       <c r="G53">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="K53"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
         <v>17</v>
       </c>
       <c r="D54" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45492.566899999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45535.696900000003</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -2422,25 +2371,24 @@
         <v>17</v>
       </c>
       <c r="G54">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="K54"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
       </c>
       <c r="D55" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44921.4211</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45030.432099999998</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -2449,25 +2397,24 @@
         <v>17</v>
       </c>
       <c r="G55">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="K55"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
       </c>
       <c r="D56" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45342.444600000003</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45210.703000000001</v>
       </c>
       <c r="E56">
         <v>2</v>
@@ -2476,25 +2423,24 @@
         <v>17</v>
       </c>
       <c r="G56">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="K56"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
         <v>17</v>
       </c>
       <c r="D57" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45361.567000000003</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45051.450400000002</v>
       </c>
       <c r="E57">
         <v>2</v>
@@ -2503,25 +2449,24 @@
         <v>17</v>
       </c>
       <c r="G57">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="K57"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
       </c>
       <c r="D58" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44868.350400000003</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45068.5988</v>
       </c>
       <c r="E58">
         <v>2</v>
@@ -2530,25 +2475,24 @@
         <v>17</v>
       </c>
       <c r="G58">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="K58"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="C59" t="s">
         <v>17</v>
       </c>
       <c r="D59" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45112.478199999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44879.553099999997</v>
       </c>
       <c r="E59">
         <v>2</v>
@@ -2557,25 +2501,24 @@
         <v>17</v>
       </c>
       <c r="G59">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="K59"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
       </c>
       <c r="D60" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45013.342499999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45364.579100000003</v>
       </c>
       <c r="E60">
         <v>2</v>
@@ -2584,25 +2527,24 @@
         <v>17</v>
       </c>
       <c r="G60">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="K60"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
         <v>17</v>
       </c>
       <c r="D61" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45148.692900000002</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45191.603199999998</v>
       </c>
       <c r="E61">
         <v>2</v>
@@ -2611,25 +2553,24 @@
         <v>17</v>
       </c>
       <c r="G61">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="K61"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
         <v>17</v>
       </c>
       <c r="D62" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45600.335099999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45224.6466</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -2638,25 +2579,24 @@
         <v>17</v>
       </c>
       <c r="G62">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="K62"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
         <v>17</v>
       </c>
       <c r="D63" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45554.400999999998</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45254.510900000001</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -2665,25 +2605,24 @@
         <v>17</v>
       </c>
       <c r="G63">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="K63"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
         <v>17</v>
       </c>
       <c r="D64" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44906.606099999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45558.671199999997</v>
       </c>
       <c r="E64">
         <v>2</v>
@@ -2692,25 +2631,24 @@
         <v>17</v>
       </c>
       <c r="G64">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="K64"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C65" t="s">
         <v>17</v>
       </c>
       <c r="D65" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45039.361499999999</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45273.539299999997</v>
       </c>
       <c r="E65">
         <v>2</v>
@@ -2719,25 +2657,24 @@
         <v>17</v>
       </c>
       <c r="G65">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="K65"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
       </c>
       <c r="D66" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45591.335200000001</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45044.659599999999</v>
       </c>
       <c r="E66">
         <v>2</v>
@@ -2746,25 +2683,24 @@
         <v>17</v>
       </c>
       <c r="G66">
-        <f t="shared" ref="G66:G99" ca="1" si="4">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="K66"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
       </c>
       <c r="D67" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45315.343999999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45210.344400000002</v>
       </c>
       <c r="E67">
         <v>2</v>
@@ -2773,25 +2709,24 @@
         <v>17</v>
       </c>
       <c r="G67">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="K67"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>44865.616199999997</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45419.376600000003</v>
       </c>
       <c r="E68">
         <v>2</v>
@@ -2800,25 +2735,24 @@
         <v>17</v>
       </c>
       <c r="G68">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="K68"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
         <v>17</v>
       </c>
       <c r="D69" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45551.66</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45395.640500000001</v>
       </c>
       <c r="E69">
         <v>2</v>
@@ -2827,25 +2761,24 @@
         <v>17</v>
       </c>
       <c r="G69">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="K69"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C70" t="s">
         <v>17</v>
       </c>
       <c r="D70" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45298.635799999996</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45593.376100000001</v>
       </c>
       <c r="E70">
         <v>2</v>
@@ -2854,25 +2787,24 @@
         <v>17</v>
       </c>
       <c r="G70">
-        <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="K70"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="C71" t="s">
         <v>17</v>
       </c>
       <c r="D71" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>45111.6564</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45038.430899999999</v>
       </c>
       <c r="E71">
         <v>2</v>
@@ -2881,25 +2813,24 @@
         <v>17</v>
       </c>
       <c r="G71">
-        <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="K71"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72">
-        <f t="shared" ref="B72:B99" ca="1" si="5">RANDBETWEEN(0,6)</f>
-        <v>2</v>
+        <f t="shared" ref="B72:B99" ca="1" si="3">RANDBETWEEN(0,6)</f>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
         <v>17</v>
       </c>
       <c r="D72" s="3">
-        <f t="shared" ref="D72:D99" ca="1" si="6">RANDBETWEEN(DATE(2022,9,31),DATE(2024,11,30))+RANDBETWEEN(TIME(8,0,0)*10000,TIME(17,0,0)*10000)/10000</f>
-        <v>45471.487800000003</v>
+        <f t="shared" ref="D72:D99" ca="1" si="4">RANDBETWEEN(DATE(2022,9,31),DATE(2024,11,30))+RANDBETWEEN(TIME(8,0,0)*10000,TIME(17,0,0)*10000)/10000</f>
+        <v>45575.456700000002</v>
       </c>
       <c r="E72">
         <v>2</v>
@@ -2908,25 +2839,24 @@
         <v>17</v>
       </c>
       <c r="G72">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="K72"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
         <v>17</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45204.547299999998</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45423.552000000003</v>
       </c>
       <c r="E73">
         <v>2</v>
@@ -2935,25 +2865,24 @@
         <v>17</v>
       </c>
       <c r="G73">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="K73"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45270.703000000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44908.385799999996</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -2962,25 +2891,24 @@
         <v>17</v>
       </c>
       <c r="G74">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="K74"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
       </c>
       <c r="C75" t="s">
         <v>17</v>
       </c>
       <c r="D75" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45463.560400000002</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45545.551899999999</v>
       </c>
       <c r="E75">
         <v>2</v>
@@ -2989,25 +2917,24 @@
         <v>17</v>
       </c>
       <c r="G75">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="K75"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
       </c>
       <c r="C76" t="s">
         <v>17</v>
       </c>
       <c r="D76" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45000.477200000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45118.655599999998</v>
       </c>
       <c r="E76">
         <v>2</v>
@@ -3016,25 +2943,24 @@
         <v>17</v>
       </c>
       <c r="G76">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="K76"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C77" t="s">
         <v>17</v>
       </c>
       <c r="D77" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>44912.680899999999</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45108.414299999997</v>
       </c>
       <c r="E77">
         <v>2</v>
@@ -3043,25 +2969,24 @@
         <v>17</v>
       </c>
       <c r="G77">
-        <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="K77"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
         <v>17</v>
       </c>
       <c r="D78" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45427.623399999997</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44837.432999999997</v>
       </c>
       <c r="E78">
         <v>2</v>
@@ -3070,25 +2995,24 @@
         <v>17</v>
       </c>
       <c r="G78">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="K78"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C79" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45422.348899999997</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45580.424599999998</v>
       </c>
       <c r="E79">
         <v>2</v>
@@ -3097,25 +3021,24 @@
         <v>17</v>
       </c>
       <c r="G79">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="K79"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="C80" t="s">
         <v>17</v>
       </c>
       <c r="D80" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45121.515200000002</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45198.5504</v>
       </c>
       <c r="E80">
         <v>2</v>
@@ -3124,25 +3047,24 @@
         <v>17</v>
       </c>
       <c r="G80">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="K80"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C81" t="s">
         <v>17</v>
       </c>
       <c r="D81" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45621.3773</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45160.3514</v>
       </c>
       <c r="E81">
         <v>2</v>
@@ -3151,25 +3073,24 @@
         <v>17</v>
       </c>
       <c r="G81">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="K81"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4</v>
       </c>
       <c r="C82" t="s">
         <v>17</v>
       </c>
       <c r="D82" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45318.690399999999</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44857.646099999998</v>
       </c>
       <c r="E82">
         <v>2</v>
@@ -3178,25 +3099,24 @@
         <v>17</v>
       </c>
       <c r="G82">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="K82"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C83" t="s">
         <v>17</v>
       </c>
       <c r="D83" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45538.371400000004</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45534.345300000001</v>
       </c>
       <c r="E83">
         <v>2</v>
@@ -3205,25 +3125,24 @@
         <v>17</v>
       </c>
       <c r="G83">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="K83"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5</v>
       </c>
       <c r="C84" t="s">
         <v>17</v>
       </c>
       <c r="D84" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45196.6633</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45516.396699999998</v>
       </c>
       <c r="E84">
         <v>2</v>
@@ -3232,25 +3151,24 @@
         <v>17</v>
       </c>
       <c r="G84">
-        <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="K84"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C85" t="s">
         <v>17</v>
       </c>
       <c r="D85" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45156.424599999998</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44938.473899999997</v>
       </c>
       <c r="E85">
         <v>2</v>
@@ -3259,25 +3177,24 @@
         <v>17</v>
       </c>
       <c r="G85">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="K85"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C86" t="s">
         <v>17</v>
       </c>
       <c r="D86" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45062.472600000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45552.519399999997</v>
       </c>
       <c r="E86">
         <v>2</v>
@@ -3286,25 +3203,24 @@
         <v>17</v>
       </c>
       <c r="G86">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="K86"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B87">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
       </c>
       <c r="C87" t="s">
         <v>17</v>
       </c>
       <c r="D87" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45604.352899999998</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45347.406999999999</v>
       </c>
       <c r="E87">
         <v>2</v>
@@ -3313,25 +3229,24 @@
         <v>17</v>
       </c>
       <c r="G87">
-        <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="K87"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
       </c>
       <c r="C88" t="s">
         <v>17</v>
       </c>
       <c r="D88" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>44956.390800000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45219.578699999998</v>
       </c>
       <c r="E88">
         <v>2</v>
@@ -3340,25 +3255,24 @@
         <v>17</v>
       </c>
       <c r="G88">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="K88"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C89" t="s">
         <v>17</v>
       </c>
       <c r="D89" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45292.573100000001</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45191.546999999999</v>
       </c>
       <c r="E89">
         <v>2</v>
@@ -3367,25 +3281,24 @@
         <v>17</v>
       </c>
       <c r="G89">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="K89"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
       </c>
       <c r="C90" t="s">
         <v>17</v>
       </c>
       <c r="D90" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45236.632400000002</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44893.380299999997</v>
       </c>
       <c r="E90">
         <v>2</v>
@@ -3394,25 +3307,24 @@
         <v>17</v>
       </c>
       <c r="G90">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="K90"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C91" t="s">
         <v>17</v>
       </c>
       <c r="D91" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45320.687700000002</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44935.622000000003</v>
       </c>
       <c r="E91">
         <v>2</v>
@@ -3421,25 +3333,24 @@
         <v>17</v>
       </c>
       <c r="G91">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="K91"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
       </c>
       <c r="C92" t="s">
         <v>17</v>
       </c>
       <c r="D92" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45405.4928</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44850.6132</v>
       </c>
       <c r="E92">
         <v>2</v>
@@ -3448,25 +3359,24 @@
         <v>17</v>
       </c>
       <c r="G92">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="K92"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
       </c>
       <c r="C93" t="s">
         <v>17</v>
       </c>
       <c r="D93" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45245.4548</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45391.653299999998</v>
       </c>
       <c r="E93">
         <v>2</v>
@@ -3475,25 +3385,24 @@
         <v>17</v>
       </c>
       <c r="G93">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="K93"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C94" t="s">
         <v>17</v>
       </c>
       <c r="D94" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45403.633800000003</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44849.651400000002</v>
       </c>
       <c r="E94">
         <v>2</v>
@@ -3502,25 +3411,24 @@
         <v>17</v>
       </c>
       <c r="G94">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="K94"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>2</v>
       </c>
       <c r="C95" t="s">
         <v>17</v>
       </c>
       <c r="D95" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>44896.509700000002</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45186.5821</v>
       </c>
       <c r="E95">
         <v>2</v>
@@ -3529,25 +3437,24 @@
         <v>17</v>
       </c>
       <c r="G95">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="K95"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
       </c>
       <c r="C96" t="s">
         <v>17</v>
       </c>
       <c r="D96" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45095.708100000003</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45162.512999999999</v>
       </c>
       <c r="E96">
         <v>2</v>
@@ -3556,25 +3463,24 @@
         <v>17</v>
       </c>
       <c r="G96">
-        <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="K96"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
       <c r="C97" t="s">
         <v>17</v>
       </c>
       <c r="D97" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45203.4323</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44922.439700000003</v>
       </c>
       <c r="E97">
         <v>2</v>
@@ -3583,25 +3489,24 @@
         <v>17</v>
       </c>
       <c r="G97">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="K97"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C98" t="s">
         <v>17</v>
       </c>
       <c r="D98" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45194.684200000003</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45181.451399999998</v>
       </c>
       <c r="E98">
         <v>2</v>
@@ -3610,25 +3515,24 @@
         <v>17</v>
       </c>
       <c r="G98">
-        <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="K98"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B99">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
       </c>
       <c r="C99" t="s">
         <v>17</v>
       </c>
       <c r="D99" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45527.589599999999</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45320.7042</v>
       </c>
       <c r="E99">
         <v>2</v>
@@ -3637,8 +3541,7 @@
         <v>17</v>
       </c>
       <c r="G99">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="K99"/>
     </row>

</xml_diff>